<commit_message>
Updated phases and CA prices
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Jupyter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="822" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13A6F5E0-D71B-4AB3-BEEC-CAAF81D86158}"/>
+  <xr:revisionPtr revIDLastSave="823" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A7F1669-42A4-4980-AA21-22B5AA10E2F6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -5656,19 +5656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>141</v>
       </c>
@@ -5702,7 +5702,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>112</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>145</v>
       </c>
@@ -5761,7 +5761,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>96</v>
       </c>
@@ -5777,7 +5777,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>97</v>
       </c>
@@ -5793,7 +5793,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>98</v>
       </c>
@@ -5809,7 +5809,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>99</v>
       </c>
@@ -5825,7 +5825,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>93</v>
       </c>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>109</v>
       </c>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>116</v>
       </c>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>91</v>
       </c>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>100</v>
       </c>
@@ -5909,7 +5909,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>173</v>
       </c>
@@ -5925,7 +5925,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>95</v>
       </c>
@@ -5941,7 +5941,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>107</v>
       </c>
@@ -5957,7 +5957,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>105</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>114</v>
       </c>
@@ -5989,7 +5989,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>106</v>
       </c>
@@ -6005,7 +6005,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>120</v>
       </c>
@@ -6020,7 +6020,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>125</v>
       </c>
@@ -6034,7 +6034,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>122</v>
       </c>
@@ -6050,7 +6050,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>117</v>
       </c>
@@ -6066,7 +6066,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>150</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>115</v>
       </c>
@@ -6096,7 +6096,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>113</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>108</v>
       </c>
@@ -6130,7 +6130,7 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>92</v>
       </c>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>90</v>
       </c>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>110</v>
       </c>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>111</v>
       </c>
@@ -6201,7 +6201,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>101</v>
       </c>
@@ -6217,7 +6217,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6234,7 +6234,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>103</v>
       </c>
@@ -6251,7 +6251,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>104</v>
       </c>
@@ -6267,46 +6267,46 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
@@ -6340,27 +6340,27 @@
       <selection pane="topRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="44" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.140625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" style="45" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="44" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" style="45" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -6451,7 +6451,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="69" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>58</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="43" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" s="43" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
@@ -6624,22 +6624,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -6653,13 +6653,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="32"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>87</v>
       </c>
@@ -6695,7 +6695,7 @@
       <c r="E4" s="70"/>
       <c r="F4" s="69"/>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
@@ -6707,13 +6707,13 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="32">
-        <f>16.05/1000</f>
-        <v>1.6050000000000002E-2</v>
+        <f>16.05/100</f>
+        <v>0.1605</v>
       </c>
       <c r="C6" s="46">
         <f>[1]Electric!$G$557/kWh_per_mmBtu</f>
@@ -6723,7 +6723,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>48</v>
       </c>
@@ -6767,13 +6767,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="32"/>
       <c r="C10" s="47"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -6801,13 +6801,13 @@
       </c>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="33"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>77</v>
       </c>
@@ -6849,26 +6849,26 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="51" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="51"/>
-    <col min="8" max="8" width="14.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="51"/>
+    <col min="8" max="8" width="14.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="13.7109375" style="51"/>
-    <col min="26" max="26" width="18.42578125" style="51" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="13.7109375" style="51"/>
+    <col min="17" max="25" width="13.6640625" style="51"/>
+    <col min="26" max="26" width="18.44140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="13.6640625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>132</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="52" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
         <v>165</v>
       </c>
@@ -6891,13 +6891,13 @@
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="F3" s="51"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>6</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>9</v>
       </c>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="D5" s="55"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
         <v>13</v>
       </c>
@@ -6949,7 +6949,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
         <v>15</v>
       </c>
@@ -6963,7 +6963,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
         <v>166</v>
       </c>
@@ -6978,7 +6978,7 @@
       <c r="F9" s="51"/>
       <c r="L9" s="51"/>
     </row>
-    <row r="10" spans="1:12" s="52" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
         <v>137</v>
       </c>
@@ -6994,7 +6994,7 @@
       <c r="F10" s="51"/>
       <c r="L10" s="51"/>
     </row>
-    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>133</v>
       </c>
@@ -7010,7 +7010,7 @@
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
     </row>
-    <row r="12" spans="1:12" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>134</v>
       </c>
@@ -7026,7 +7026,7 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -7034,10 +7034,10 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="52"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>138</v>
       </c>
@@ -7058,7 +7058,7 @@
       <c r="O17" s="72"/>
       <c r="P17" s="72"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="71" t="s">
         <v>129</v>
       </c>
@@ -7088,7 +7088,7 @@
       <c r="O18" s="71"/>
       <c r="P18" s="71"/>
     </row>
-    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="57" t="s">
         <v>167</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="61">
         <v>-51.5244564886654</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="61">
         <v>-89.797974315320403</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="61">
         <v>-128.06720097650799</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="61">
         <v>-166.34194485043901</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="61">
         <v>-204.613623606179</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="61">
         <v>-242.881624220091</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="61">
         <v>-281.15268995219299</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="61">
         <v>-319.427433826124</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="61">
         <v>-357.69420839275898</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="61">
         <v>-395.96343505394702</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="61">
         <v>-434.23572683332497</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="61">
         <v>-472.50188837632197</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="61">
         <v>-510.774180155701</v>
       </c>
@@ -7851,7 +7851,7 @@
       <c r="O32" s="63"/>
       <c r="P32" s="63"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="61">
         <v>-549.04095472233598</v>
       </c>
@@ -7894,7 +7894,7 @@
       <c r="O33" s="63"/>
       <c r="P33" s="63"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="61">
         <v>-587.30895533624698</v>
       </c>
@@ -7937,7 +7937,7 @@
       <c r="O34" s="63"/>
       <c r="P34" s="63"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="61">
         <v>-625.57511687924398</v>
       </c>
@@ -7980,7 +7980,7 @@
       <c r="O35" s="63"/>
       <c r="P35" s="63"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="61">
         <v>-663.84066539860203</v>
       </c>
@@ -8023,7 +8023,7 @@
       <c r="O36" s="63"/>
       <c r="P36" s="63"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="61">
         <v>-702.104987870684</v>
       </c>
@@ -8066,7 +8066,7 @@
       <c r="O37" s="63"/>
       <c r="P37" s="63"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="61">
         <v>-740.36747127185197</v>
       </c>
@@ -8109,7 +8109,7 @@
       <c r="O38" s="63"/>
       <c r="P38" s="63"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="61">
         <v>-778.62934164938099</v>
       </c>
@@ -8152,7 +8152,7 @@
       <c r="O39" s="63"/>
       <c r="P39" s="63"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="61">
         <v>-816.88814690872005</v>
       </c>
@@ -8195,7 +8195,7 @@
       <c r="O40" s="63"/>
       <c r="P40" s="63"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="61">
         <v>-855.14633914442004</v>
       </c>
@@ -8238,7 +8238,7 @@
       <c r="O41" s="63"/>
       <c r="P41" s="63"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="61">
         <v>-893.40453138012003</v>
       </c>
@@ -8281,7 +8281,7 @@
       <c r="O42" s="63"/>
       <c r="P42" s="63"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="61">
         <v>-931.65781942671504</v>
       </c>
@@ -8324,7 +8324,7 @@
       <c r="O43" s="63"/>
       <c r="P43" s="63"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="61">
         <v>-969.90988142603396</v>
       </c>
@@ -8367,7 +8367,7 @@
       <c r="O44" s="63"/>
       <c r="P44" s="63"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="61">
         <v>-1008.15397411805</v>
       </c>
@@ -8410,7 +8410,7 @@
       <c r="O45" s="63"/>
       <c r="P45" s="63"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="61">
         <v>-1046.3962277391599</v>
       </c>
@@ -8453,7 +8453,7 @@
       <c r="O46" s="63"/>
       <c r="P46" s="63"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="61">
         <v>-1084.6305120529701</v>
       </c>
@@ -8496,7 +8496,7 @@
       <c r="O47" s="63"/>
       <c r="P47" s="63"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="61">
         <v>-1122.8660224140599</v>
       </c>
@@ -8526,7 +8526,7 @@
       <c r="O48" s="63"/>
       <c r="P48" s="63"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="61">
         <v>-1161.08743323147</v>
       </c>
@@ -8556,7 +8556,7 @@
       <c r="O49" s="63"/>
       <c r="P49" s="63"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="61">
         <v>-1199.30516590705</v>
       </c>
@@ -8586,7 +8586,7 @@
       <c r="O50" s="63"/>
       <c r="P50" s="63"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="61">
         <v>-1237.5192204407999</v>
       </c>
@@ -8616,7 +8616,7 @@
       <c r="O51" s="63"/>
       <c r="P51" s="63"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="61">
         <v>-1275.72530566725</v>
       </c>
@@ -8646,7 +8646,7 @@
       <c r="O52" s="63"/>
       <c r="P52" s="63"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="61">
         <v>-1313.9283257755101</v>
       </c>
@@ -8676,7 +8676,7 @@
       <c r="O53" s="63"/>
       <c r="P53" s="63"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="61">
         <v>-1352.1258286710299</v>
       </c>
@@ -8706,7 +8706,7 @@
       <c r="O54" s="63"/>
       <c r="P54" s="63"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="61">
         <v>-1390.3306878502101</v>
       </c>
@@ -8736,7 +8736,7 @@
       <c r="O55" s="63"/>
       <c r="P55" s="63"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="61">
         <v>-1428.5300298166501</v>
       </c>
@@ -8766,7 +8766,7 @@
       <c r="O56" s="63"/>
       <c r="P56" s="63"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="61">
         <v>-1466.7189503812299</v>
       </c>
@@ -8796,7 +8796,7 @@
       <c r="O57" s="63"/>
       <c r="P57" s="63"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="61">
         <v>-1499.6968635093899</v>
       </c>
@@ -8826,7 +8826,7 @@
       <c r="O58" s="63"/>
       <c r="P58" s="63"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J62" s="65"/>
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
@@ -8835,7 +8835,7 @@
       <c r="O62" s="51"/>
       <c r="P62" s="51"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H63" s="71" t="s">
         <v>132</v>
       </c>
@@ -8848,7 +8848,7 @@
       <c r="O63" s="51"/>
       <c r="P63" s="51"/>
     </row>
-    <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
       <c r="H64" s="66" t="s">
         <v>169</v>
       </c>
@@ -8863,7 +8863,7 @@
       <c r="O64" s="51"/>
       <c r="P64" s="51"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H65" s="67">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -8879,7 +8879,7 @@
       <c r="O65" s="51"/>
       <c r="P65" s="51"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H66" s="67">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -8895,7 +8895,7 @@
       <c r="O66" s="51"/>
       <c r="P66" s="51"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H67" s="67">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -8911,7 +8911,7 @@
       <c r="O67" s="51"/>
       <c r="P67" s="51"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H68" s="67">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -8927,7 +8927,7 @@
       <c r="O68" s="51"/>
       <c r="P68" s="51"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H69" s="67">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -8943,7 +8943,7 @@
       <c r="O69" s="51"/>
       <c r="P69" s="51"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H70" s="67">
         <v>0.1080445517892699</v>
       </c>
@@ -8959,7 +8959,7 @@
       <c r="O70" s="51"/>
       <c r="P70" s="51"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H71" s="67">
         <v>0.12497606826753388</v>
       </c>
@@ -8975,7 +8975,7 @@
       <c r="O71" s="51"/>
       <c r="P71" s="51"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H72" s="67">
         <v>0.14198052165390951</v>
       </c>
@@ -8991,7 +8991,7 @@
       <c r="O72" s="51"/>
       <c r="P72" s="51"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H73" s="67">
         <v>0.15874470475517963</v>
       </c>
@@ -9007,7 +9007,7 @@
       <c r="O73" s="51"/>
       <c r="P73" s="51"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H74" s="67">
         <v>0.17553747925232432</v>
       </c>
@@ -9023,7 +9023,7 @@
       <c r="O74" s="51"/>
       <c r="P74" s="51"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H75" s="67">
         <v>0.19240417629290971</v>
       </c>
@@ -9039,7 +9039,7 @@
       <c r="O75" s="51"/>
       <c r="P75" s="51"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H76" s="67">
         <v>0.20901220546271423</v>
       </c>
@@ -9055,7 +9055,7 @@
       <c r="O76" s="51"/>
       <c r="P76" s="51"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H77" s="67">
         <v>0.22582431925537669</v>
       </c>
@@ -9071,7 +9071,7 @@
       <c r="O77" s="51"/>
       <c r="P77" s="51"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H78" s="67">
         <v>0.24236713011424937</v>
       </c>
@@ -9087,7 +9087,7 @@
       <c r="O78" s="51"/>
       <c r="P78" s="51"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H79" s="67">
         <v>0.25891734586657894</v>
       </c>
@@ -9103,7 +9103,7 @@
       <c r="O79" s="51"/>
       <c r="P79" s="51"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H80" s="67">
         <v>0.27532743679881172</v>
       </c>
@@ -9119,7 +9119,7 @@
       <c r="O80" s="51"/>
       <c r="P80" s="51"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H81" s="67">
         <v>0.29164753874763422</v>
       </c>
@@ -9135,7 +9135,7 @@
       <c r="O81" s="51"/>
       <c r="P81" s="51"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H82" s="67">
         <v>0.30783618288424536</v>
       </c>
@@ -9151,7 +9151,7 @@
       <c r="O82" s="51"/>
       <c r="P82" s="51"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H83" s="67">
         <v>0.32384418347196781</v>
       </c>
@@ -9167,7 +9167,7 @@
       <c r="O83" s="51"/>
       <c r="P83" s="51"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H84" s="67">
         <v>0.33973325501759533</v>
       </c>
@@ -9183,7 +9183,7 @@
       <c r="O84" s="51"/>
       <c r="P84" s="51"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H85" s="67">
         <v>0.3553317399203158</v>
       </c>
@@ -9199,7 +9199,7 @@
       <c r="O85" s="51"/>
       <c r="P85" s="51"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H86" s="67">
         <v>0.37078429028268828</v>
       </c>
@@ -9215,7 +9215,7 @@
       <c r="O86" s="51"/>
       <c r="P86" s="51"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H87" s="67">
         <v>0.38613044476352726</v>
       </c>
@@ -9231,7 +9231,7 @@
       <c r="O87" s="51"/>
       <c r="P87" s="51"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H88" s="67">
         <v>0.4009921758963842</v>
       </c>
@@ -9247,7 +9247,7 @@
       <c r="O88" s="51"/>
       <c r="P88" s="51"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H89" s="67">
         <v>0.4156182923872962</v>
       </c>
@@ -9263,7 +9263,7 @@
       <c r="O89" s="51"/>
       <c r="P89" s="51"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H90" s="67">
         <v>0.42943502667027428</v>
       </c>
@@ -9279,7 +9279,7 @@
       <c r="O90" s="51"/>
       <c r="P90" s="51"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H91" s="67">
         <v>0.44289756776749095</v>
       </c>
@@ -9295,7 +9295,7 @@
       <c r="O91" s="51"/>
       <c r="P91" s="51"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H92" s="67">
         <v>0.45543894715911687</v>
       </c>
@@ -9311,7 +9311,7 @@
       <c r="O92" s="51"/>
       <c r="P92" s="51"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H93" s="67">
         <v>0.46783735943015631</v>
       </c>
@@ -9327,7 +9327,7 @@
       <c r="O93" s="51"/>
       <c r="P93" s="51"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H94" s="67">
         <v>0.47863400366300879</v>
       </c>
@@ -9343,7 +9343,7 @@
       <c r="O94" s="51"/>
       <c r="P94" s="51"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H95" s="67">
         <v>0.48872859410433517</v>
       </c>
@@ -9359,7 +9359,7 @@
       <c r="O95" s="51"/>
       <c r="P95" s="51"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H96" s="67">
         <v>0.49808648675762501</v>
       </c>
@@ -9375,7 +9375,7 @@
       <c r="O96" s="51"/>
       <c r="P96" s="51"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H97" s="67">
         <v>0.50622094031681064</v>
       </c>
@@ -9391,7 +9391,7 @@
       <c r="O97" s="51"/>
       <c r="P97" s="51"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H98" s="67">
         <v>0.51358901063162188</v>
       </c>
@@ -9407,7 +9407,7 @@
       <c r="O98" s="51"/>
       <c r="P98" s="51"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H99" s="67">
         <v>0.51988812196851808</v>
       </c>
@@ -9423,7 +9423,7 @@
       <c r="O99" s="51"/>
       <c r="P99" s="51"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H100" s="67">
         <v>0.52654380991188665</v>
       </c>
@@ -9439,7 +9439,7 @@
       <c r="O100" s="51"/>
       <c r="P100" s="51"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H101" s="67">
         <v>0.53210746291493216</v>
       </c>
@@ -9455,7 +9455,7 @@
       <c r="O101" s="51"/>
       <c r="P101" s="51"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H102" s="67">
         <v>0.53593356457098895</v>
       </c>
@@ -9471,7 +9471,7 @@
       <c r="O102" s="51"/>
       <c r="P102" s="51"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H103" s="67">
         <v>0.53837802652041589</v>
       </c>
@@ -9487,7 +9487,7 @@
       <c r="O103" s="51"/>
       <c r="P103" s="51"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
       <c r="K104" s="51"/>
       <c r="L104" s="51"/>
       <c r="M104" s="51"/>

</xml_diff>

<commit_message>
Updated default total emissions
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="823" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A7F1669-42A4-4980-AA21-22B5AA10E2F6}"/>
+  <xr:revisionPtr revIDLastSave="838" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2A2EFB5-BF81-4FEE-9A55-5F5A105D9189}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -5656,19 +5656,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>141</v>
       </c>
@@ -5702,7 +5702,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>112</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>145</v>
       </c>
@@ -5761,7 +5761,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>96</v>
       </c>
@@ -5777,7 +5777,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>97</v>
       </c>
@@ -5793,7 +5793,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>98</v>
       </c>
@@ -5809,7 +5809,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>99</v>
       </c>
@@ -5825,7 +5825,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>93</v>
       </c>
@@ -5841,7 +5841,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>109</v>
       </c>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>116</v>
       </c>
@@ -5875,7 +5875,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>91</v>
       </c>
@@ -5893,7 +5893,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>100</v>
       </c>
@@ -5909,7 +5909,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>173</v>
       </c>
@@ -5925,7 +5925,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>95</v>
       </c>
@@ -5941,7 +5941,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>107</v>
       </c>
@@ -5957,7 +5957,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>105</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>114</v>
       </c>
@@ -5989,7 +5989,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>106</v>
       </c>
@@ -6005,7 +6005,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>120</v>
       </c>
@@ -6020,7 +6020,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>125</v>
       </c>
@@ -6034,7 +6034,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>122</v>
       </c>
@@ -6050,7 +6050,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>117</v>
       </c>
@@ -6066,7 +6066,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>150</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>115</v>
       </c>
@@ -6096,7 +6096,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>113</v>
       </c>
@@ -6112,7 +6112,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>108</v>
       </c>
@@ -6130,7 +6130,7 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>92</v>
       </c>
@@ -6148,7 +6148,7 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>90</v>
       </c>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>110</v>
       </c>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>111</v>
       </c>
@@ -6201,7 +6201,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>101</v>
       </c>
@@ -6217,7 +6217,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6234,7 +6234,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>103</v>
       </c>
@@ -6251,7 +6251,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>104</v>
       </c>
@@ -6267,46 +6267,46 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
@@ -6337,30 +6337,30 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="44" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" style="45" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="4"/>
+    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="44" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" style="45" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -6451,7 +6451,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="69" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -6505,7 +6505,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>58</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="43" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="43" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
@@ -6624,22 +6624,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -6653,13 +6653,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="32"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>87</v>
       </c>
@@ -6695,7 +6695,7 @@
       <c r="E4" s="70"/>
       <c r="F4" s="69"/>
     </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
@@ -6707,7 +6707,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -6723,7 +6723,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>48</v>
       </c>
@@ -6767,13 +6767,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="32"/>
       <c r="C10" s="47"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -6801,13 +6801,13 @@
       </c>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="33"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>77</v>
       </c>
@@ -6849,26 +6849,26 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="51" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="51"/>
-    <col min="8" max="8" width="14.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="51"/>
+    <col min="8" max="8" width="14.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="13.6640625" style="51"/>
-    <col min="26" max="26" width="18.44140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="13.6640625" style="51"/>
+    <col min="17" max="25" width="13.7109375" style="51"/>
+    <col min="26" max="26" width="18.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="13.7109375" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
         <v>132</v>
       </c>
@@ -6879,7 +6879,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="52" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
         <v>165</v>
       </c>
@@ -6891,13 +6891,13 @@
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="F3" s="51"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>6</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>9</v>
       </c>
@@ -6923,7 +6923,7 @@
       </c>
       <c r="D5" s="55"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
@@ -6935,7 +6935,7 @@
       </c>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
         <v>13</v>
       </c>
@@ -6949,7 +6949,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
         <v>15</v>
       </c>
@@ -6963,7 +6963,7 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
         <v>166</v>
       </c>
@@ -6978,7 +6978,7 @@
       <c r="F9" s="51"/>
       <c r="L9" s="51"/>
     </row>
-    <row r="10" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="52" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
         <v>137</v>
       </c>
@@ -6994,7 +6994,7 @@
       <c r="F10" s="51"/>
       <c r="L10" s="51"/>
     </row>
-    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
         <v>133</v>
       </c>
@@ -7010,7 +7010,7 @@
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
     </row>
-    <row r="12" spans="1:12" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
         <v>134</v>
       </c>
@@ -7026,7 +7026,7 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -7034,10 +7034,10 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="52"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="72" t="s">
         <v>138</v>
       </c>
@@ -7058,7 +7058,7 @@
       <c r="O17" s="72"/>
       <c r="P17" s="72"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="s">
         <v>129</v>
       </c>
@@ -7088,7 +7088,7 @@
       <c r="O18" s="71"/>
       <c r="P18" s="71"/>
     </row>
-    <row r="19" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="57" t="s">
         <v>167</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="61">
         <v>-51.5244564886654</v>
       </c>
@@ -7192,7 +7192,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="61">
         <v>-89.797974315320403</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="61">
         <v>-128.06720097650799</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="61">
         <v>-166.34194485043901</v>
       </c>
@@ -7360,7 +7360,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="61">
         <v>-204.613623606179</v>
       </c>
@@ -7416,7 +7416,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="61">
         <v>-242.881624220091</v>
       </c>
@@ -7472,7 +7472,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="61">
         <v>-281.15268995219299</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="61">
         <v>-319.427433826124</v>
       </c>
@@ -7584,7 +7584,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="61">
         <v>-357.69420839275898</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="61">
         <v>-395.96343505394702</v>
       </c>
@@ -7696,7 +7696,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="61">
         <v>-434.23572683332497</v>
       </c>
@@ -7752,7 +7752,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="61">
         <v>-472.50188837632197</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="61">
         <v>-510.774180155701</v>
       </c>
@@ -7851,7 +7851,7 @@
       <c r="O32" s="63"/>
       <c r="P32" s="63"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="61">
         <v>-549.04095472233598</v>
       </c>
@@ -7894,7 +7894,7 @@
       <c r="O33" s="63"/>
       <c r="P33" s="63"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="61">
         <v>-587.30895533624698</v>
       </c>
@@ -7937,7 +7937,7 @@
       <c r="O34" s="63"/>
       <c r="P34" s="63"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="61">
         <v>-625.57511687924398</v>
       </c>
@@ -7980,7 +7980,7 @@
       <c r="O35" s="63"/>
       <c r="P35" s="63"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="61">
         <v>-663.84066539860203</v>
       </c>
@@ -8023,7 +8023,7 @@
       <c r="O36" s="63"/>
       <c r="P36" s="63"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="61">
         <v>-702.104987870684</v>
       </c>
@@ -8066,7 +8066,7 @@
       <c r="O37" s="63"/>
       <c r="P37" s="63"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="61">
         <v>-740.36747127185197</v>
       </c>
@@ -8109,7 +8109,7 @@
       <c r="O38" s="63"/>
       <c r="P38" s="63"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="61">
         <v>-778.62934164938099</v>
       </c>
@@ -8152,7 +8152,7 @@
       <c r="O39" s="63"/>
       <c r="P39" s="63"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="61">
         <v>-816.88814690872005</v>
       </c>
@@ -8195,7 +8195,7 @@
       <c r="O40" s="63"/>
       <c r="P40" s="63"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="61">
         <v>-855.14633914442004</v>
       </c>
@@ -8238,7 +8238,7 @@
       <c r="O41" s="63"/>
       <c r="P41" s="63"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="61">
         <v>-893.40453138012003</v>
       </c>
@@ -8281,7 +8281,7 @@
       <c r="O42" s="63"/>
       <c r="P42" s="63"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="61">
         <v>-931.65781942671504</v>
       </c>
@@ -8324,7 +8324,7 @@
       <c r="O43" s="63"/>
       <c r="P43" s="63"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="61">
         <v>-969.90988142603396</v>
       </c>
@@ -8367,7 +8367,7 @@
       <c r="O44" s="63"/>
       <c r="P44" s="63"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="61">
         <v>-1008.15397411805</v>
       </c>
@@ -8410,7 +8410,7 @@
       <c r="O45" s="63"/>
       <c r="P45" s="63"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="61">
         <v>-1046.3962277391599</v>
       </c>
@@ -8453,7 +8453,7 @@
       <c r="O46" s="63"/>
       <c r="P46" s="63"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="61">
         <v>-1084.6305120529701</v>
       </c>
@@ -8496,7 +8496,7 @@
       <c r="O47" s="63"/>
       <c r="P47" s="63"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="61">
         <v>-1122.8660224140599</v>
       </c>
@@ -8526,7 +8526,7 @@
       <c r="O48" s="63"/>
       <c r="P48" s="63"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="61">
         <v>-1161.08743323147</v>
       </c>
@@ -8556,7 +8556,7 @@
       <c r="O49" s="63"/>
       <c r="P49" s="63"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="61">
         <v>-1199.30516590705</v>
       </c>
@@ -8586,7 +8586,7 @@
       <c r="O50" s="63"/>
       <c r="P50" s="63"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="61">
         <v>-1237.5192204407999</v>
       </c>
@@ -8616,7 +8616,7 @@
       <c r="O51" s="63"/>
       <c r="P51" s="63"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="61">
         <v>-1275.72530566725</v>
       </c>
@@ -8646,7 +8646,7 @@
       <c r="O52" s="63"/>
       <c r="P52" s="63"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="61">
         <v>-1313.9283257755101</v>
       </c>
@@ -8676,7 +8676,7 @@
       <c r="O53" s="63"/>
       <c r="P53" s="63"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="61">
         <v>-1352.1258286710299</v>
       </c>
@@ -8706,7 +8706,7 @@
       <c r="O54" s="63"/>
       <c r="P54" s="63"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="61">
         <v>-1390.3306878502101</v>
       </c>
@@ -8736,7 +8736,7 @@
       <c r="O55" s="63"/>
       <c r="P55" s="63"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="61">
         <v>-1428.5300298166501</v>
       </c>
@@ -8766,7 +8766,7 @@
       <c r="O56" s="63"/>
       <c r="P56" s="63"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="61">
         <v>-1466.7189503812299</v>
       </c>
@@ -8796,7 +8796,7 @@
       <c r="O57" s="63"/>
       <c r="P57" s="63"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="61">
         <v>-1499.6968635093899</v>
       </c>
@@ -8826,7 +8826,7 @@
       <c r="O58" s="63"/>
       <c r="P58" s="63"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J62" s="65"/>
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
@@ -8835,7 +8835,7 @@
       <c r="O62" s="51"/>
       <c r="P62" s="51"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H63" s="71" t="s">
         <v>132</v>
       </c>
@@ -8848,7 +8848,7 @@
       <c r="O63" s="51"/>
       <c r="P63" s="51"/>
     </row>
-    <row r="64" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="H64" s="66" t="s">
         <v>169</v>
       </c>
@@ -8863,7 +8863,7 @@
       <c r="O64" s="51"/>
       <c r="P64" s="51"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H65" s="67">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -8879,7 +8879,7 @@
       <c r="O65" s="51"/>
       <c r="P65" s="51"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H66" s="67">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -8895,7 +8895,7 @@
       <c r="O66" s="51"/>
       <c r="P66" s="51"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H67" s="67">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -8911,7 +8911,7 @@
       <c r="O67" s="51"/>
       <c r="P67" s="51"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H68" s="67">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -8927,7 +8927,7 @@
       <c r="O68" s="51"/>
       <c r="P68" s="51"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H69" s="67">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -8943,7 +8943,7 @@
       <c r="O69" s="51"/>
       <c r="P69" s="51"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H70" s="67">
         <v>0.1080445517892699</v>
       </c>
@@ -8959,7 +8959,7 @@
       <c r="O70" s="51"/>
       <c r="P70" s="51"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H71" s="67">
         <v>0.12497606826753388</v>
       </c>
@@ -8975,7 +8975,7 @@
       <c r="O71" s="51"/>
       <c r="P71" s="51"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H72" s="67">
         <v>0.14198052165390951</v>
       </c>
@@ -8991,7 +8991,7 @@
       <c r="O72" s="51"/>
       <c r="P72" s="51"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H73" s="67">
         <v>0.15874470475517963</v>
       </c>
@@ -9007,7 +9007,7 @@
       <c r="O73" s="51"/>
       <c r="P73" s="51"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H74" s="67">
         <v>0.17553747925232432</v>
       </c>
@@ -9023,7 +9023,7 @@
       <c r="O74" s="51"/>
       <c r="P74" s="51"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H75" s="67">
         <v>0.19240417629290971</v>
       </c>
@@ -9039,7 +9039,7 @@
       <c r="O75" s="51"/>
       <c r="P75" s="51"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H76" s="67">
         <v>0.20901220546271423</v>
       </c>
@@ -9055,7 +9055,7 @@
       <c r="O76" s="51"/>
       <c r="P76" s="51"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H77" s="67">
         <v>0.22582431925537669</v>
       </c>
@@ -9071,7 +9071,7 @@
       <c r="O77" s="51"/>
       <c r="P77" s="51"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H78" s="67">
         <v>0.24236713011424937</v>
       </c>
@@ -9087,7 +9087,7 @@
       <c r="O78" s="51"/>
       <c r="P78" s="51"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H79" s="67">
         <v>0.25891734586657894</v>
       </c>
@@ -9103,7 +9103,7 @@
       <c r="O79" s="51"/>
       <c r="P79" s="51"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H80" s="67">
         <v>0.27532743679881172</v>
       </c>
@@ -9119,7 +9119,7 @@
       <c r="O80" s="51"/>
       <c r="P80" s="51"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H81" s="67">
         <v>0.29164753874763422</v>
       </c>
@@ -9135,7 +9135,7 @@
       <c r="O81" s="51"/>
       <c r="P81" s="51"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H82" s="67">
         <v>0.30783618288424536</v>
       </c>
@@ -9151,7 +9151,7 @@
       <c r="O82" s="51"/>
       <c r="P82" s="51"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H83" s="67">
         <v>0.32384418347196781</v>
       </c>
@@ -9167,7 +9167,7 @@
       <c r="O83" s="51"/>
       <c r="P83" s="51"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H84" s="67">
         <v>0.33973325501759533</v>
       </c>
@@ -9183,7 +9183,7 @@
       <c r="O84" s="51"/>
       <c r="P84" s="51"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H85" s="67">
         <v>0.3553317399203158</v>
       </c>
@@ -9199,7 +9199,7 @@
       <c r="O85" s="51"/>
       <c r="P85" s="51"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H86" s="67">
         <v>0.37078429028268828</v>
       </c>
@@ -9215,7 +9215,7 @@
       <c r="O86" s="51"/>
       <c r="P86" s="51"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H87" s="67">
         <v>0.38613044476352726</v>
       </c>
@@ -9231,7 +9231,7 @@
       <c r="O87" s="51"/>
       <c r="P87" s="51"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H88" s="67">
         <v>0.4009921758963842</v>
       </c>
@@ -9247,7 +9247,7 @@
       <c r="O88" s="51"/>
       <c r="P88" s="51"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H89" s="67">
         <v>0.4156182923872962</v>
       </c>
@@ -9263,7 +9263,7 @@
       <c r="O89" s="51"/>
       <c r="P89" s="51"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H90" s="67">
         <v>0.42943502667027428</v>
       </c>
@@ -9279,7 +9279,7 @@
       <c r="O90" s="51"/>
       <c r="P90" s="51"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H91" s="67">
         <v>0.44289756776749095</v>
       </c>
@@ -9295,7 +9295,7 @@
       <c r="O91" s="51"/>
       <c r="P91" s="51"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H92" s="67">
         <v>0.45543894715911687</v>
       </c>
@@ -9311,7 +9311,7 @@
       <c r="O92" s="51"/>
       <c r="P92" s="51"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H93" s="67">
         <v>0.46783735943015631</v>
       </c>
@@ -9327,7 +9327,7 @@
       <c r="O93" s="51"/>
       <c r="P93" s="51"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H94" s="67">
         <v>0.47863400366300879</v>
       </c>
@@ -9343,7 +9343,7 @@
       <c r="O94" s="51"/>
       <c r="P94" s="51"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H95" s="67">
         <v>0.48872859410433517</v>
       </c>
@@ -9359,7 +9359,7 @@
       <c r="O95" s="51"/>
       <c r="P95" s="51"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H96" s="67">
         <v>0.49808648675762501</v>
       </c>
@@ -9375,7 +9375,7 @@
       <c r="O96" s="51"/>
       <c r="P96" s="51"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H97" s="67">
         <v>0.50622094031681064</v>
       </c>
@@ -9391,7 +9391,7 @@
       <c r="O97" s="51"/>
       <c r="P97" s="51"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H98" s="67">
         <v>0.51358901063162188</v>
       </c>
@@ -9407,7 +9407,7 @@
       <c r="O98" s="51"/>
       <c r="P98" s="51"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H99" s="67">
         <v>0.51988812196851808</v>
       </c>
@@ -9423,7 +9423,7 @@
       <c r="O99" s="51"/>
       <c r="P99" s="51"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H100" s="67">
         <v>0.52654380991188665</v>
       </c>
@@ -9439,7 +9439,7 @@
       <c r="O100" s="51"/>
       <c r="P100" s="51"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H101" s="67">
         <v>0.53210746291493216</v>
       </c>
@@ -9455,7 +9455,7 @@
       <c r="O101" s="51"/>
       <c r="P101" s="51"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H102" s="67">
         <v>0.53593356457098895</v>
       </c>
@@ -9471,7 +9471,7 @@
       <c r="O102" s="51"/>
       <c r="P102" s="51"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H103" s="67">
         <v>0.53837802652041589</v>
       </c>
@@ -9487,7 +9487,7 @@
       <c r="O103" s="51"/>
       <c r="P103" s="51"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K104" s="51"/>
       <c r="L104" s="51"/>
       <c r="M104" s="51"/>

</xml_diff>

<commit_message>
Updated electricity price (first half of 2024), electrolyzer and PSA capex (CEPCI 2024), CO price (adjusted to 2024)
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="845" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{014D1E41-CCDD-4602-AAAC-E660701DF1C2}"/>
+  <xr:revisionPtr revIDLastSave="859" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FD5C09-DE53-4AA7-A0F1-CDD05D54B5B3}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="3840" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="176">
   <si>
     <t>Utility</t>
   </si>
@@ -901,9 +901,6 @@
     <t>Badgett, Cortright (J. Cleaner Prod. 2022)</t>
   </si>
   <si>
-    <t>George (Kirk-Othmer Encyclopedia 2001); but $0.1 (syngas?) in Guerra, Hodge (Joule, 2023)</t>
-  </si>
-  <si>
     <t>Nitopi, Jaramillo (Chem. Rev. 2019)</t>
   </si>
   <si>
@@ -1048,7 +1045,17 @@
     <t>Gas constant</t>
   </si>
   <si>
-    <t>Average 2017 - 2023 from Krungsri Research and Bloomberg via Statista</t>
+    <t>U.S. Energy Information Administration (Jan - Jun 2024) - industrial retail; GREET (2022)</t>
+  </si>
+  <si>
+    <t>CEPCI 2021: 773.1
+CEPCI 2024: 800</t>
+  </si>
+  <si>
+    <t>Average 2024 from Krungsri Research and Bloomberg via Statista</t>
+  </si>
+  <si>
+    <t>George (Kirk-Othmer Encyclopedia 2001) adjusted by 1% inflation; but $0.1 (syngas?) in Guerra, Hodge (Joule, 2023)</t>
   </si>
 </sst>
 </file>
@@ -5656,19 +5663,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF78F5ED-8DF7-423A-A030-17DE1F110F66}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -5686,7 +5693,7 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>141</v>
       </c>
@@ -5702,7 +5709,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
@@ -5722,7 +5729,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>112</v>
       </c>
@@ -5743,7 +5750,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>145</v>
       </c>
@@ -5751,7 +5758,8 @@
         <v>146</v>
       </c>
       <c r="C5" s="35">
-        <v>5000</v>
+        <f>5000*800/773.1</f>
+        <v>5173.9749062217043</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>147</v>
@@ -5759,9 +5767,11 @@
       <c r="E5" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="F5" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>96</v>
       </c>
@@ -5777,7 +5787,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>97</v>
       </c>
@@ -5793,7 +5803,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>98</v>
       </c>
@@ -5809,7 +5819,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>99</v>
       </c>
@@ -5825,7 +5835,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>93</v>
       </c>
@@ -5841,7 +5851,7 @@
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>109</v>
       </c>
@@ -5857,7 +5867,7 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>116</v>
       </c>
@@ -5875,7 +5885,7 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>91</v>
       </c>
@@ -5893,7 +5903,7 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>100</v>
       </c>
@@ -5909,9 +5919,9 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>9</v>
@@ -5925,7 +5935,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>95</v>
       </c>
@@ -5941,7 +5951,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>107</v>
       </c>
@@ -5957,7 +5967,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>105</v>
       </c>
@@ -5973,7 +5983,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>114</v>
       </c>
@@ -5989,7 +5999,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>106</v>
       </c>
@@ -6005,7 +6015,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>120</v>
       </c>
@@ -6020,7 +6030,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>125</v>
       </c>
@@ -6034,7 +6044,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>122</v>
       </c>
@@ -6050,7 +6060,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>117</v>
       </c>
@@ -6066,7 +6076,7 @@
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>150</v>
       </c>
@@ -6082,7 +6092,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>115</v>
       </c>
@@ -6096,7 +6106,7 @@
       <c r="E26" s="24"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>113</v>
       </c>
@@ -6112,7 +6122,7 @@
       <c r="E27" s="24"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>108</v>
       </c>
@@ -6130,7 +6140,7 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>92</v>
       </c>
@@ -6148,7 +6158,7 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>90</v>
       </c>
@@ -6167,7 +6177,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>110</v>
       </c>
@@ -6185,7 +6195,7 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>111</v>
       </c>
@@ -6201,7 +6211,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>101</v>
       </c>
@@ -6217,7 +6227,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6234,7 +6244,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>103</v>
       </c>
@@ -6251,7 +6261,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>104</v>
       </c>
@@ -6267,46 +6277,46 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
@@ -6335,32 +6345,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="44" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.140625" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" style="4" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" style="45" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="44" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="4" customWidth="1"/>
+    <col min="17" max="17" width="20.88671875" style="45" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
@@ -6413,7 +6423,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -6451,7 +6461,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -6471,7 +6481,8 @@
         <v>10160</v>
       </c>
       <c r="G3" s="9">
-        <v>0.6</v>
+        <f>0.6*(1.015^(2024-2001))</f>
+        <v>0.84502629276592345</v>
       </c>
       <c r="H3" s="10">
         <v>-0.06</v>
@@ -6502,10 +6513,10 @@
         <v>20</v>
       </c>
       <c r="Q3" s="42" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="71.25" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>58</v>
       </c>
@@ -6525,8 +6536,8 @@
         <v>47741</v>
       </c>
       <c r="G4" s="9">
-        <f>958.71/1000</f>
-        <v>0.95871000000000006</v>
+        <f>AVERAGE(880,955,1010,1005,969,966,921,947,954)/1000</f>
+        <v>0.95633333333333337</v>
       </c>
       <c r="H4" s="6">
         <v>0.09</v>
@@ -6556,10 +6567,10 @@
         <v>20</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="43" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="43" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
@@ -6570,7 +6581,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>71</v>
@@ -6582,10 +6593,10 @@
         <v>76</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J5" s="27" t="s">
         <v>61</v>
@@ -6612,7 +6623,7 @@
     <hyperlink ref="I5" r:id="rId5" display="Nitopi Jaramillo Chem Rev 2019" xr:uid="{15A9F7F2-24C4-4947-B8AC-CCED0C43AB79}"/>
     <hyperlink ref="P4" r:id="rId6" xr:uid="{9E5C44A6-93F6-4ED1-B804-8649E4167F70}"/>
     <hyperlink ref="Q3" r:id="rId7" display="Jouny, Jiao I&amp;EC 2018" xr:uid="{10B5C8FC-32D4-41B8-BAEB-C077AC9722AB}"/>
-    <hyperlink ref="Q4" r:id="rId8" xr:uid="{1CA02CE1-315F-432C-AD96-D17BF918BC72}"/>
+    <hyperlink ref="Q4" r:id="rId8" display="Average 2017 - 2023 from Krungsri Research and Bloomberg via Statista" xr:uid="{1CA02CE1-315F-432C-AD96-D17BF918BC72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId9"/>
@@ -6626,22 +6637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -6655,13 +6666,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17"/>
       <c r="B2" s="32"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -6672,16 +6683,16 @@
         <v>50</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="69" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>87</v>
       </c>
@@ -6692,12 +6703,12 @@
         <v>20</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" s="70"/>
       <c r="F4" s="69"/>
     </row>
-    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>86</v>
       </c>
@@ -6706,10 +6717,10 @@
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="30" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -6722,26 +6733,26 @@
         <v>230.93061430996579</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="32">
-        <f>7.62/100</f>
-        <v>7.6200000000000004E-2</v>
+        <f>8.19/100</f>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="C7" s="46" cm="1">
         <f t="array" ref="C7">[1]!Electricity_upstream_fuel_CO2/kWh_per_mmBtu</f>
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -6754,10 +6765,10 @@
         <v>254.376</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>48</v>
       </c>
@@ -6769,19 +6780,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="32"/>
       <c r="C10" s="47"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="32">
         <f>B7</f>
-        <v>7.6200000000000004E-2</v>
+        <v>8.1900000000000001E-2</v>
       </c>
       <c r="C11" s="47">
         <f>C7</f>
@@ -6789,7 +6800,7 @@
       </c>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -6803,13 +6814,13 @@
       </c>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="20"/>
       <c r="B13" s="33"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>77</v>
       </c>
@@ -6833,7 +6844,7 @@
     <hyperlink ref="D14" r:id="rId4" xr:uid="{AE632364-779F-4089-A88D-F487214F42B4}"/>
     <hyperlink ref="D4" r:id="rId5" display="Lazard April 2023; GREET 2022" xr:uid="{001DDBDA-9A42-4028-A4C3-DD34E948B14B}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{EEDCFB93-E59F-403A-99E8-154836C00872}"/>
-    <hyperlink ref="D7" r:id="rId7" xr:uid="{2B223392-32B3-448A-811F-60ABD0999D47}"/>
+    <hyperlink ref="D7" r:id="rId7" display="U.S. Energy Information Administration (April 2023) - industrial retail; GREET (2022)" xr:uid="{2B223392-32B3-448A-811F-60ABD0999D47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -6851,26 +6862,26 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="51" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="51"/>
-    <col min="8" max="8" width="14.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" style="52" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="51"/>
+    <col min="8" max="8" width="14.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.44140625" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="13.7109375" style="51"/>
-    <col min="26" max="26" width="18.42578125" style="51" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="13.7109375" style="51"/>
+    <col min="17" max="25" width="13.6640625" style="51"/>
+    <col min="26" max="26" width="18.44140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="13.6640625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="48" t="s">
         <v>132</v>
       </c>
@@ -6878,28 +6889,28 @@
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
       <c r="E1" s="51" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="52" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="50"/>
       <c r="D2" s="50"/>
       <c r="E2" s="68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="F3" s="51"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="53" t="s">
         <v>6</v>
       </c>
@@ -6913,7 +6924,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>9</v>
       </c>
@@ -6925,7 +6936,7 @@
       </c>
       <c r="D5" s="55"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
@@ -6937,7 +6948,7 @@
       </c>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="55" t="s">
         <v>13</v>
       </c>
@@ -6951,7 +6962,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="56" t="s">
         <v>15</v>
       </c>
@@ -6965,9 +6976,9 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9" s="55">
         <v>273.14999999999998</v>
@@ -6980,7 +6991,7 @@
       <c r="F9" s="51"/>
       <c r="L9" s="51"/>
     </row>
-    <row r="10" spans="1:12" s="52" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="56" t="s">
         <v>137</v>
       </c>
@@ -6996,7 +7007,7 @@
       <c r="F10" s="51"/>
       <c r="L10" s="51"/>
     </row>
-    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>133</v>
       </c>
@@ -7012,7 +7023,7 @@
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
     </row>
-    <row r="12" spans="1:12" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>134</v>
       </c>
@@ -7028,7 +7039,7 @@
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -7036,10 +7047,10 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="52"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="72" t="s">
         <v>138</v>
       </c>
@@ -7060,7 +7071,7 @@
       <c r="O17" s="72"/>
       <c r="P17" s="72"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="71" t="s">
         <v>129</v>
       </c>
@@ -7090,55 +7101,55 @@
       <c r="O18" s="71"/>
       <c r="P18" s="71"/>
     </row>
-    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="B19" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="B19" s="57" t="s">
-        <v>167</v>
-      </c>
       <c r="C19" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="D19" s="57" t="s">
-        <v>167</v>
-      </c>
       <c r="E19" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="57" t="s">
         <v>166</v>
-      </c>
-      <c r="F19" s="57" t="s">
-        <v>167</v>
       </c>
       <c r="G19" s="58"/>
       <c r="H19" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="I19" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="I19" s="59" t="s">
+      <c r="J19" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="J19" s="60" t="s">
-        <v>169</v>
-      </c>
       <c r="K19" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="L19" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="L19" s="59" t="s">
+      <c r="M19" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="M19" s="60" t="s">
-        <v>169</v>
-      </c>
       <c r="N19" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="O19" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="O19" s="59" t="s">
+      <c r="P19" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="P19" s="60" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="61">
         <v>-51.5244564886654</v>
       </c>
@@ -7194,7 +7205,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="61">
         <v>-89.797974315320403</v>
       </c>
@@ -7250,7 +7261,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="61">
         <v>-128.06720097650799</v>
       </c>
@@ -7306,7 +7317,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="61">
         <v>-166.34194485043901</v>
       </c>
@@ -7362,7 +7373,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="61">
         <v>-204.613623606179</v>
       </c>
@@ -7418,7 +7429,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="61">
         <v>-242.881624220091</v>
       </c>
@@ -7474,7 +7485,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="61">
         <v>-281.15268995219299</v>
       </c>
@@ -7530,7 +7541,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="61">
         <v>-319.427433826124</v>
       </c>
@@ -7586,7 +7597,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="61">
         <v>-357.69420839275898</v>
       </c>
@@ -7642,7 +7653,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="61">
         <v>-395.96343505394702</v>
       </c>
@@ -7698,7 +7709,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="61">
         <v>-434.23572683332497</v>
       </c>
@@ -7754,7 +7765,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="61">
         <v>-472.50188837632197</v>
       </c>
@@ -7810,7 +7821,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="61">
         <v>-510.774180155701</v>
       </c>
@@ -7853,7 +7864,7 @@
       <c r="O32" s="63"/>
       <c r="P32" s="63"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="61">
         <v>-549.04095472233598</v>
       </c>
@@ -7896,7 +7907,7 @@
       <c r="O33" s="63"/>
       <c r="P33" s="63"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="61">
         <v>-587.30895533624698</v>
       </c>
@@ -7939,7 +7950,7 @@
       <c r="O34" s="63"/>
       <c r="P34" s="63"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="61">
         <v>-625.57511687924398</v>
       </c>
@@ -7982,7 +7993,7 @@
       <c r="O35" s="63"/>
       <c r="P35" s="63"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="61">
         <v>-663.84066539860203</v>
       </c>
@@ -8025,7 +8036,7 @@
       <c r="O36" s="63"/>
       <c r="P36" s="63"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="61">
         <v>-702.104987870684</v>
       </c>
@@ -8068,7 +8079,7 @@
       <c r="O37" s="63"/>
       <c r="P37" s="63"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="61">
         <v>-740.36747127185197</v>
       </c>
@@ -8111,7 +8122,7 @@
       <c r="O38" s="63"/>
       <c r="P38" s="63"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="61">
         <v>-778.62934164938099</v>
       </c>
@@ -8154,7 +8165,7 @@
       <c r="O39" s="63"/>
       <c r="P39" s="63"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="61">
         <v>-816.88814690872005</v>
       </c>
@@ -8197,7 +8208,7 @@
       <c r="O40" s="63"/>
       <c r="P40" s="63"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="61">
         <v>-855.14633914442004</v>
       </c>
@@ -8240,7 +8251,7 @@
       <c r="O41" s="63"/>
       <c r="P41" s="63"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="61">
         <v>-893.40453138012003</v>
       </c>
@@ -8283,7 +8294,7 @@
       <c r="O42" s="63"/>
       <c r="P42" s="63"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="61">
         <v>-931.65781942671504</v>
       </c>
@@ -8326,7 +8337,7 @@
       <c r="O43" s="63"/>
       <c r="P43" s="63"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="61">
         <v>-969.90988142603396</v>
       </c>
@@ -8369,7 +8380,7 @@
       <c r="O44" s="63"/>
       <c r="P44" s="63"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="61">
         <v>-1008.15397411805</v>
       </c>
@@ -8412,7 +8423,7 @@
       <c r="O45" s="63"/>
       <c r="P45" s="63"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="61">
         <v>-1046.3962277391599</v>
       </c>
@@ -8455,7 +8466,7 @@
       <c r="O46" s="63"/>
       <c r="P46" s="63"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="61">
         <v>-1084.6305120529701</v>
       </c>
@@ -8498,7 +8509,7 @@
       <c r="O47" s="63"/>
       <c r="P47" s="63"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="61">
         <v>-1122.8660224140599</v>
       </c>
@@ -8528,7 +8539,7 @@
       <c r="O48" s="63"/>
       <c r="P48" s="63"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="61">
         <v>-1161.08743323147</v>
       </c>
@@ -8558,7 +8569,7 @@
       <c r="O49" s="63"/>
       <c r="P49" s="63"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="61">
         <v>-1199.30516590705</v>
       </c>
@@ -8588,7 +8599,7 @@
       <c r="O50" s="63"/>
       <c r="P50" s="63"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="61">
         <v>-1237.5192204407999</v>
       </c>
@@ -8618,7 +8629,7 @@
       <c r="O51" s="63"/>
       <c r="P51" s="63"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="61">
         <v>-1275.72530566725</v>
       </c>
@@ -8648,7 +8659,7 @@
       <c r="O52" s="63"/>
       <c r="P52" s="63"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="61">
         <v>-1313.9283257755101</v>
       </c>
@@ -8678,7 +8689,7 @@
       <c r="O53" s="63"/>
       <c r="P53" s="63"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="61">
         <v>-1352.1258286710299</v>
       </c>
@@ -8708,7 +8719,7 @@
       <c r="O54" s="63"/>
       <c r="P54" s="63"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="61">
         <v>-1390.3306878502101</v>
       </c>
@@ -8738,7 +8749,7 @@
       <c r="O55" s="63"/>
       <c r="P55" s="63"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="61">
         <v>-1428.5300298166501</v>
       </c>
@@ -8768,7 +8779,7 @@
       <c r="O56" s="63"/>
       <c r="P56" s="63"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="61">
         <v>-1466.7189503812299</v>
       </c>
@@ -8798,7 +8809,7 @@
       <c r="O57" s="63"/>
       <c r="P57" s="63"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="61">
         <v>-1499.6968635093899</v>
       </c>
@@ -8828,7 +8839,7 @@
       <c r="O58" s="63"/>
       <c r="P58" s="63"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J62" s="65"/>
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
@@ -8837,7 +8848,7 @@
       <c r="O62" s="51"/>
       <c r="P62" s="51"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H63" s="71" t="s">
         <v>132</v>
       </c>
@@ -8850,12 +8861,12 @@
       <c r="O63" s="51"/>
       <c r="P63" s="51"/>
     </row>
-    <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
       <c r="H64" s="66" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I64" s="66" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J64" s="51"/>
       <c r="K64" s="51"/>
@@ -8865,7 +8876,7 @@
       <c r="O64" s="51"/>
       <c r="P64" s="51"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H65" s="67">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -8881,7 +8892,7 @@
       <c r="O65" s="51"/>
       <c r="P65" s="51"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H66" s="67">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -8897,7 +8908,7 @@
       <c r="O66" s="51"/>
       <c r="P66" s="51"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H67" s="67">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -8913,7 +8924,7 @@
       <c r="O67" s="51"/>
       <c r="P67" s="51"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H68" s="67">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -8929,7 +8940,7 @@
       <c r="O68" s="51"/>
       <c r="P68" s="51"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H69" s="67">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -8945,7 +8956,7 @@
       <c r="O69" s="51"/>
       <c r="P69" s="51"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H70" s="67">
         <v>0.1080445517892699</v>
       </c>
@@ -8961,7 +8972,7 @@
       <c r="O70" s="51"/>
       <c r="P70" s="51"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H71" s="67">
         <v>0.12497606826753388</v>
       </c>
@@ -8977,7 +8988,7 @@
       <c r="O71" s="51"/>
       <c r="P71" s="51"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H72" s="67">
         <v>0.14198052165390951</v>
       </c>
@@ -8993,7 +9004,7 @@
       <c r="O72" s="51"/>
       <c r="P72" s="51"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H73" s="67">
         <v>0.15874470475517963</v>
       </c>
@@ -9009,7 +9020,7 @@
       <c r="O73" s="51"/>
       <c r="P73" s="51"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H74" s="67">
         <v>0.17553747925232432</v>
       </c>
@@ -9025,7 +9036,7 @@
       <c r="O74" s="51"/>
       <c r="P74" s="51"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H75" s="67">
         <v>0.19240417629290971</v>
       </c>
@@ -9041,7 +9052,7 @@
       <c r="O75" s="51"/>
       <c r="P75" s="51"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H76" s="67">
         <v>0.20901220546271423</v>
       </c>
@@ -9057,7 +9068,7 @@
       <c r="O76" s="51"/>
       <c r="P76" s="51"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H77" s="67">
         <v>0.22582431925537669</v>
       </c>
@@ -9073,7 +9084,7 @@
       <c r="O77" s="51"/>
       <c r="P77" s="51"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H78" s="67">
         <v>0.24236713011424937</v>
       </c>
@@ -9089,7 +9100,7 @@
       <c r="O78" s="51"/>
       <c r="P78" s="51"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H79" s="67">
         <v>0.25891734586657894</v>
       </c>
@@ -9105,7 +9116,7 @@
       <c r="O79" s="51"/>
       <c r="P79" s="51"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H80" s="67">
         <v>0.27532743679881172</v>
       </c>
@@ -9121,7 +9132,7 @@
       <c r="O80" s="51"/>
       <c r="P80" s="51"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H81" s="67">
         <v>0.29164753874763422</v>
       </c>
@@ -9137,7 +9148,7 @@
       <c r="O81" s="51"/>
       <c r="P81" s="51"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H82" s="67">
         <v>0.30783618288424536</v>
       </c>
@@ -9153,7 +9164,7 @@
       <c r="O82" s="51"/>
       <c r="P82" s="51"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H83" s="67">
         <v>0.32384418347196781</v>
       </c>
@@ -9169,7 +9180,7 @@
       <c r="O83" s="51"/>
       <c r="P83" s="51"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H84" s="67">
         <v>0.33973325501759533</v>
       </c>
@@ -9185,7 +9196,7 @@
       <c r="O84" s="51"/>
       <c r="P84" s="51"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H85" s="67">
         <v>0.3553317399203158</v>
       </c>
@@ -9201,7 +9212,7 @@
       <c r="O85" s="51"/>
       <c r="P85" s="51"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H86" s="67">
         <v>0.37078429028268828</v>
       </c>
@@ -9217,7 +9228,7 @@
       <c r="O86" s="51"/>
       <c r="P86" s="51"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H87" s="67">
         <v>0.38613044476352726</v>
       </c>
@@ -9233,7 +9244,7 @@
       <c r="O87" s="51"/>
       <c r="P87" s="51"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H88" s="67">
         <v>0.4009921758963842</v>
       </c>
@@ -9249,7 +9260,7 @@
       <c r="O88" s="51"/>
       <c r="P88" s="51"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H89" s="67">
         <v>0.4156182923872962</v>
       </c>
@@ -9265,7 +9276,7 @@
       <c r="O89" s="51"/>
       <c r="P89" s="51"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H90" s="67">
         <v>0.42943502667027428</v>
       </c>
@@ -9281,7 +9292,7 @@
       <c r="O90" s="51"/>
       <c r="P90" s="51"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H91" s="67">
         <v>0.44289756776749095</v>
       </c>
@@ -9297,7 +9308,7 @@
       <c r="O91" s="51"/>
       <c r="P91" s="51"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H92" s="67">
         <v>0.45543894715911687</v>
       </c>
@@ -9313,7 +9324,7 @@
       <c r="O92" s="51"/>
       <c r="P92" s="51"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H93" s="67">
         <v>0.46783735943015631</v>
       </c>
@@ -9329,7 +9340,7 @@
       <c r="O93" s="51"/>
       <c r="P93" s="51"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H94" s="67">
         <v>0.47863400366300879</v>
       </c>
@@ -9345,7 +9356,7 @@
       <c r="O94" s="51"/>
       <c r="P94" s="51"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H95" s="67">
         <v>0.48872859410433517</v>
       </c>
@@ -9361,7 +9372,7 @@
       <c r="O95" s="51"/>
       <c r="P95" s="51"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H96" s="67">
         <v>0.49808648675762501</v>
       </c>
@@ -9377,7 +9388,7 @@
       <c r="O96" s="51"/>
       <c r="P96" s="51"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H97" s="67">
         <v>0.50622094031681064</v>
       </c>
@@ -9393,7 +9404,7 @@
       <c r="O97" s="51"/>
       <c r="P97" s="51"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H98" s="67">
         <v>0.51358901063162188</v>
       </c>
@@ -9409,7 +9420,7 @@
       <c r="O98" s="51"/>
       <c r="P98" s="51"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H99" s="67">
         <v>0.51988812196851808</v>
       </c>
@@ -9425,7 +9436,7 @@
       <c r="O99" s="51"/>
       <c r="P99" s="51"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H100" s="67">
         <v>0.52654380991188665</v>
       </c>
@@ -9441,7 +9452,7 @@
       <c r="O100" s="51"/>
       <c r="P100" s="51"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H101" s="67">
         <v>0.53210746291493216</v>
       </c>
@@ -9457,7 +9468,7 @@
       <c r="O101" s="51"/>
       <c r="P101" s="51"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H102" s="67">
         <v>0.53593356457098895</v>
       </c>
@@ -9473,7 +9484,7 @@
       <c r="O102" s="51"/>
       <c r="P102" s="51"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
       <c r="H103" s="67">
         <v>0.53837802652041589</v>
       </c>
@@ -9489,7 +9500,7 @@
       <c r="O103" s="51"/>
       <c r="P103" s="51"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
       <c r="K104" s="51"/>
       <c r="L104" s="51"/>
       <c r="M104" s="51"/>

</xml_diff>

<commit_message>
Optimized j_total and SPC for new costs
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Jupyter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="859" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6FD5C09-DE53-4AA7-A0F1-CDD05D54B5B3}"/>
+  <xr:revisionPtr revIDLastSave="867" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9447385-82B6-485D-A010-CC88D5C41EBC}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -582,12 +582,6 @@
     <t>electrolyte_conc</t>
   </si>
   <si>
-    <t>Optimal SPC @ 7.6 c/kWh, Hawks model</t>
-  </si>
-  <si>
-    <t>Optimal j @ 7.6 c/kWh, Hawks model</t>
-  </si>
-  <si>
     <t>Electricity - wind + storage</t>
   </si>
   <si>
@@ -1056,6 +1050,12 @@
   </si>
   <si>
     <t>George (Kirk-Othmer Encyclopedia 2001) adjusted by 1% inflation; but $0.1 (syngas?) in Guerra, Hodge (Joule, 2023)</t>
+  </si>
+  <si>
+    <t>Optimal SPC @ 8.2 c/kWh, Hawks model</t>
+  </si>
+  <si>
+    <t>Optimal j @ 8.2 c/kWh, Hawks model</t>
   </si>
 </sst>
 </file>
@@ -4749,8 +4749,8 @@
     <tableColumn id="8" xr3:uid="{63FE646D-E5BD-46A5-B63F-54D7C89DFC20}" name="Tafel slope (mV/dec)" dataDxfId="21"/>
     <tableColumn id="7" xr3:uid="{8762D60F-6494-4D48-BF71-09EE6526135E}" name="Reference current density (mA/cm2)" dataDxfId="20"/>
     <tableColumn id="15" xr3:uid="{C96EBEF2-D837-4395-8D46-7E2BC536E261}" name="FECO2R at SPC = 0" dataDxfId="19"/>
-    <tableColumn id="16" xr3:uid="{F3E3F633-1F65-481C-8C36-D0FBD783D2AB}" name="Optimal SPC @ 7.6 c/kWh, Hawks model" dataDxfId="18"/>
-    <tableColumn id="17" xr3:uid="{06806002-8BCC-442F-99A4-15A00506143C}" name="Optimal j @ 7.6 c/kWh, Hawks model" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{F3E3F633-1F65-481C-8C36-D0FBD783D2AB}" name="Optimal SPC @ 8.2 c/kWh, Hawks model" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{06806002-8BCC-442F-99A4-15A00506143C}" name="Optimal j @ 8.2 c/kWh, Hawks model" dataDxfId="17"/>
     <tableColumn id="4" xr3:uid="{EA53ED90-0A02-4FC0-8D2F-B62ACD3411A0}" name="References" dataDxfId="16"/>
     <tableColumn id="10" xr3:uid="{15AF80F1-11B7-4792-895F-6EC0B2B7A7A4}" name="References 2" dataDxfId="15"/>
   </tableColumns>
@@ -5667,15 +5667,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.88671875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="25.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.85546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -5693,9 +5693,9 @@
       </c>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>83</v>
@@ -5709,9 +5709,9 @@
       <c r="E2" s="24"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>74</v>
@@ -5723,57 +5723,57 @@
         <v>75</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="39">
         <f>0.0145</f>
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E4" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>146</v>
       </c>
       <c r="C5" s="35">
         <f>5000*800/773.1</f>
         <v>5173.9749062217043</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>33</v>
@@ -5787,9 +5787,9 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>35</v>
@@ -5803,9 +5803,9 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>34</v>
@@ -5819,9 +5819,9 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>50</v>
@@ -5835,25 +5835,25 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="11">
         <v>0.9</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>72</v>
@@ -5867,9 +5867,9 @@
       </c>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>45</v>
@@ -5885,9 +5885,9 @@
       </c>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>36</v>
@@ -5903,9 +5903,9 @@
       </c>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>11</v>
@@ -5919,9 +5919,9 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>9</v>
@@ -5935,9 +5935,9 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>46</v>
@@ -5951,9 +5951,9 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>79</v>
@@ -5967,9 +5967,9 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>49</v>
@@ -5983,9 +5983,9 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>47</v>
@@ -5999,9 +5999,9 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>15</v>
@@ -6015,12 +6015,12 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C21" s="11">
         <f>350/365</f>
@@ -6030,12 +6030,12 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" s="29">
         <v>0</v>
@@ -6044,57 +6044,57 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C23" s="36">
         <v>20</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C24" s="35">
         <v>50000</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C25" s="35">
         <v>5</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>81</v>
@@ -6106,9 +6106,9 @@
       <c r="E26" s="24"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>80</v>
@@ -6117,14 +6117,14 @@
         <v>2500</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>39</v>
@@ -6140,9 +6140,9 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>37</v>
@@ -6158,9 +6158,9 @@
       </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>38</v>
@@ -6170,16 +6170,16 @@
         <v>41</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>20</v>
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>40</v>
@@ -6195,12 +6195,12 @@
       </c>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C32" s="10">
         <v>313.14999999999998</v>
@@ -6211,9 +6211,9 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>41</v>
@@ -6227,9 +6227,9 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>42</v>
@@ -6244,9 +6244,9 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>44</v>
@@ -6261,9 +6261,9 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>43</v>
@@ -6277,46 +6277,46 @@
       </c>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
       <c r="B46" s="8"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
@@ -6345,32 +6345,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="4" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="44" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="15.109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="20.88671875" style="45" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="4"/>
+    <col min="4" max="4" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="44" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="15.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" style="45" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="58.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>53</v>
       </c>
@@ -6411,10 +6411,10 @@
         <v>78</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>84</v>
+        <v>174</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>24</v>
@@ -6423,7 +6423,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>62</v>
       </c>
@@ -6461,7 +6461,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" ht="82.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="99.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>52</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>0.95</v>
       </c>
       <c r="N3" s="40">
-        <v>0.1148</v>
+        <v>0.12379999999999999</v>
       </c>
       <c r="O3" s="41">
         <v>472.1</v>
@@ -6513,10 +6513,10 @@
         <v>20</v>
       </c>
       <c r="Q3" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="55.2" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>58</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>0.7</v>
       </c>
       <c r="N4" s="40">
-        <v>2.6550000000000001E-2</v>
+        <v>2.9170000000000001E-2</v>
       </c>
       <c r="O4" s="41">
         <v>435.9</v>
@@ -6567,10 +6567,10 @@
         <v>20</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" s="43" customFormat="1" ht="55.2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" s="43" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>24</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>71</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>71</v>
@@ -6593,10 +6593,10 @@
         <v>76</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J5" s="27" t="s">
         <v>61</v>
@@ -6637,22 +6637,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -6666,13 +6666,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17"/>
       <c r="B2" s="32"/>
       <c r="C2" s="21"/>
       <c r="D2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>5</v>
       </c>
@@ -6683,18 +6683,18 @@
         <v>50</v>
       </c>
       <c r="D3" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="70" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="70" t="s">
-        <v>159</v>
-      </c>
       <c r="F3" s="69" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B4" s="32">
         <v>2.4E-2</v>
@@ -6703,24 +6703,24 @@
         <v>20</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E4" s="70"/>
       <c r="F4" s="69"/>
     </row>
-    <row r="5" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="32">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
@@ -6733,10 +6733,10 @@
         <v>230.93061430996579</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
@@ -6749,10 +6749,10 @@
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="69" x14ac:dyDescent="0.3">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>3</v>
       </c>
@@ -6765,10 +6765,10 @@
         <v>254.376</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>48</v>
       </c>
@@ -6780,13 +6780,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="32"/>
       <c r="C10" s="47"/>
       <c r="D10" s="37"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>25</v>
       </c>
@@ -6800,7 +6800,7 @@
       </c>
       <c r="D11" s="37"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>26</v>
       </c>
@@ -6814,13 +6814,13 @@
       </c>
       <c r="D12" s="37"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="33"/>
       <c r="C13" s="37"/>
       <c r="D13" s="37"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>77</v>
       </c>
@@ -6829,7 +6829,7 @@
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -6862,55 +6862,55 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" style="51" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" style="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="51" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" style="51" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="51"/>
-    <col min="8" max="8" width="14.6640625" style="51" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="14.6640625" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="51"/>
+    <col min="8" max="8" width="14.7109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="14.7109375" style="52" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" style="52" bestFit="1" customWidth="1"/>
-    <col min="17" max="25" width="13.6640625" style="51"/>
-    <col min="26" max="26" width="18.44140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="13.6640625" style="51"/>
+    <col min="17" max="25" width="13.7109375" style="51"/>
+    <col min="26" max="26" width="18.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="13.7109375" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="48" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B1" s="49"/>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
       <c r="E1" s="51" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="52" customFormat="1" ht="16.2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A2" s="48" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="50"/>
       <c r="D2" s="50"/>
       <c r="E2" s="68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F2" s="51"/>
     </row>
-    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="51"/>
       <c r="C3" s="51"/>
       <c r="D3" s="51"/>
       <c r="F3" s="51"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="53" t="s">
         <v>6</v>
       </c>
@@ -6921,10 +6921,10 @@
         <v>8</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>9</v>
       </c>
@@ -6936,7 +6936,7 @@
       </c>
       <c r="D5" s="55"/>
     </row>
-    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="56" t="s">
         <v>11</v>
       </c>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
         <v>13</v>
       </c>
@@ -6962,7 +6962,7 @@
       <c r="E7" s="51"/>
       <c r="F7" s="51"/>
     </row>
-    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="56" t="s">
         <v>15</v>
       </c>
@@ -6976,9 +6976,9 @@
       <c r="E8" s="51"/>
       <c r="F8" s="51"/>
     </row>
-    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="55">
         <v>273.14999999999998</v>
@@ -6991,55 +6991,55 @@
       <c r="F9" s="51"/>
       <c r="L9" s="51"/>
     </row>
-    <row r="10" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="52" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B10" s="56">
         <f>1/60/(100^3)*P/(R_*B7+20)</f>
         <v>7.3709198831561756E-7</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D10" s="56"/>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="L10" s="51"/>
     </row>
-    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="55" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B11" s="55">
         <f>1/60/(100^3)*P/(R_*B7)</f>
         <v>7.4358305104930494E-7</v>
       </c>
       <c r="C11" s="55" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D11" s="55"/>
       <c r="E11" s="51"/>
       <c r="F11" s="51"/>
       <c r="G11" s="51"/>
     </row>
-    <row r="12" spans="1:12" s="52" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="56" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B12" s="56">
         <f>1/(1000*2*F)</f>
         <v>5.182134828131088E-9</v>
       </c>
       <c r="C12" s="56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="51"/>
       <c r="F12" s="51"/>
       <c r="G12" s="51"/>
     </row>
-    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="51"/>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -7047,12 +7047,12 @@
       <c r="F13" s="51"/>
       <c r="G13" s="51"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="52"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="72" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" s="72"/>
       <c r="C17" s="72"/>
@@ -7060,7 +7060,7 @@
       <c r="E17" s="72"/>
       <c r="F17" s="72"/>
       <c r="H17" s="72" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I17" s="72"/>
       <c r="J17" s="72"/>
@@ -7071,85 +7071,85 @@
       <c r="O17" s="72"/>
       <c r="P17" s="72"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B18" s="71"/>
       <c r="C18" s="71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D18" s="71"/>
       <c r="E18" s="71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F18" s="71"/>
       <c r="G18" s="58"/>
       <c r="H18" s="71" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I18" s="71"/>
       <c r="J18" s="71"/>
       <c r="K18" s="71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L18" s="71"/>
       <c r="M18" s="71"/>
       <c r="N18" s="71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="O18" s="71"/>
       <c r="P18" s="71"/>
     </row>
-    <row r="19" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F19" s="57" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G19" s="58"/>
       <c r="H19" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="I19" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="I19" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="J19" s="60" t="s">
-        <v>168</v>
-      </c>
       <c r="K19" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="L19" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="M19" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="L19" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="M19" s="60" t="s">
-        <v>168</v>
-      </c>
       <c r="N19" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="O19" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="P19" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="O19" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="P19" s="60" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="61">
         <v>-51.5244564886654</v>
       </c>
@@ -7205,7 +7205,7 @@
         <v>5.0730403065140095E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="61">
         <v>-89.797974315320403</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>6.5460850237780699E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="61">
         <v>-128.06720097650799</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>8.6704673566159185E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="61">
         <v>-166.34194485043901</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>1.1771856112818058E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="61">
         <v>-204.613623606179</v>
       </c>
@@ -7429,7 +7429,7 @@
         <v>1.6610145177220037E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="61">
         <v>-242.881624220091</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>2.2533996934247069E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="61">
         <v>-281.15268995219299</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>3.149742423062496E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="61">
         <v>-319.427433826124</v>
       </c>
@@ -7597,7 +7597,7 @@
         <v>4.8494015452431039E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="61">
         <v>-357.69420839275898</v>
       </c>
@@ -7653,7 +7653,7 @@
         <v>7.7219536858392002E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="61">
         <v>-395.96343505394702</v>
       </c>
@@ -7709,7 +7709,7 @@
         <v>0.10626191485734104</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="61">
         <v>-434.23572683332497</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>-1.8498964897695203E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="61">
         <v>-472.50188837632197</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>-1.3483050770102256E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="61">
         <v>-510.774180155701</v>
       </c>
@@ -7864,7 +7864,7 @@
       <c r="O32" s="63"/>
       <c r="P32" s="63"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="61">
         <v>-549.04095472233598</v>
       </c>
@@ -7907,7 +7907,7 @@
       <c r="O33" s="63"/>
       <c r="P33" s="63"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="61">
         <v>-587.30895533624698</v>
       </c>
@@ -7950,7 +7950,7 @@
       <c r="O34" s="63"/>
       <c r="P34" s="63"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="61">
         <v>-625.57511687924398</v>
       </c>
@@ -7993,7 +7993,7 @@
       <c r="O35" s="63"/>
       <c r="P35" s="63"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="61">
         <v>-663.84066539860203</v>
       </c>
@@ -8036,7 +8036,7 @@
       <c r="O36" s="63"/>
       <c r="P36" s="63"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="61">
         <v>-702.104987870684</v>
       </c>
@@ -8079,7 +8079,7 @@
       <c r="O37" s="63"/>
       <c r="P37" s="63"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="61">
         <v>-740.36747127185197</v>
       </c>
@@ -8122,7 +8122,7 @@
       <c r="O38" s="63"/>
       <c r="P38" s="63"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="61">
         <v>-778.62934164938099</v>
       </c>
@@ -8165,7 +8165,7 @@
       <c r="O39" s="63"/>
       <c r="P39" s="63"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="61">
         <v>-816.88814690872005</v>
       </c>
@@ -8208,7 +8208,7 @@
       <c r="O40" s="63"/>
       <c r="P40" s="63"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="61">
         <v>-855.14633914442004</v>
       </c>
@@ -8251,7 +8251,7 @@
       <c r="O41" s="63"/>
       <c r="P41" s="63"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="61">
         <v>-893.40453138012003</v>
       </c>
@@ -8294,7 +8294,7 @@
       <c r="O42" s="63"/>
       <c r="P42" s="63"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="61">
         <v>-931.65781942671504</v>
       </c>
@@ -8337,7 +8337,7 @@
       <c r="O43" s="63"/>
       <c r="P43" s="63"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="61">
         <v>-969.90988142603396</v>
       </c>
@@ -8380,7 +8380,7 @@
       <c r="O44" s="63"/>
       <c r="P44" s="63"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="61">
         <v>-1008.15397411805</v>
       </c>
@@ -8423,7 +8423,7 @@
       <c r="O45" s="63"/>
       <c r="P45" s="63"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="61">
         <v>-1046.3962277391599</v>
       </c>
@@ -8466,7 +8466,7 @@
       <c r="O46" s="63"/>
       <c r="P46" s="63"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="61">
         <v>-1084.6305120529701</v>
       </c>
@@ -8509,7 +8509,7 @@
       <c r="O47" s="63"/>
       <c r="P47" s="63"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="61">
         <v>-1122.8660224140599</v>
       </c>
@@ -8539,7 +8539,7 @@
       <c r="O48" s="63"/>
       <c r="P48" s="63"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="61">
         <v>-1161.08743323147</v>
       </c>
@@ -8569,7 +8569,7 @@
       <c r="O49" s="63"/>
       <c r="P49" s="63"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" s="61">
         <v>-1199.30516590705</v>
       </c>
@@ -8599,7 +8599,7 @@
       <c r="O50" s="63"/>
       <c r="P50" s="63"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" s="61">
         <v>-1237.5192204407999</v>
       </c>
@@ -8629,7 +8629,7 @@
       <c r="O51" s="63"/>
       <c r="P51" s="63"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="61">
         <v>-1275.72530566725</v>
       </c>
@@ -8659,7 +8659,7 @@
       <c r="O52" s="63"/>
       <c r="P52" s="63"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" s="61">
         <v>-1313.9283257755101</v>
       </c>
@@ -8689,7 +8689,7 @@
       <c r="O53" s="63"/>
       <c r="P53" s="63"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" s="61">
         <v>-1352.1258286710299</v>
       </c>
@@ -8719,7 +8719,7 @@
       <c r="O54" s="63"/>
       <c r="P54" s="63"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="61">
         <v>-1390.3306878502101</v>
       </c>
@@ -8749,7 +8749,7 @@
       <c r="O55" s="63"/>
       <c r="P55" s="63"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="61">
         <v>-1428.5300298166501</v>
       </c>
@@ -8779,7 +8779,7 @@
       <c r="O56" s="63"/>
       <c r="P56" s="63"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="61">
         <v>-1466.7189503812299</v>
       </c>
@@ -8809,7 +8809,7 @@
       <c r="O57" s="63"/>
       <c r="P57" s="63"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="61">
         <v>-1499.6968635093899</v>
       </c>
@@ -8839,7 +8839,7 @@
       <c r="O58" s="63"/>
       <c r="P58" s="63"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="J62" s="65"/>
       <c r="K62" s="51"/>
       <c r="L62" s="51"/>
@@ -8848,9 +8848,9 @@
       <c r="O62" s="51"/>
       <c r="P62" s="51"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H63" s="71" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I63" s="71"/>
       <c r="J63" s="65"/>
@@ -8861,12 +8861,12 @@
       <c r="O63" s="51"/>
       <c r="P63" s="51"/>
     </row>
-    <row r="64" spans="1:16" ht="16.2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="H64" s="66" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I64" s="66" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J64" s="51"/>
       <c r="K64" s="51"/>
@@ -8876,7 +8876,7 @@
       <c r="O64" s="51"/>
       <c r="P64" s="51"/>
     </row>
-    <row r="65" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H65" s="67">
         <v>2.2997934048565084E-2</v>
       </c>
@@ -8892,7 +8892,7 @@
       <c r="O65" s="51"/>
       <c r="P65" s="51"/>
     </row>
-    <row r="66" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H66" s="67">
         <v>4.0069676396611777E-2</v>
       </c>
@@ -8908,7 +8908,7 @@
       <c r="O66" s="51"/>
       <c r="P66" s="51"/>
     </row>
-    <row r="67" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H67" s="67">
         <v>5.7084370034302737E-2</v>
       </c>
@@ -8924,7 +8924,7 @@
       <c r="O67" s="51"/>
       <c r="P67" s="51"/>
     </row>
-    <row r="68" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H68" s="67">
         <v>7.4140086301005395E-2</v>
       </c>
@@ -8940,7 +8940,7 @@
       <c r="O68" s="51"/>
       <c r="P68" s="51"/>
     </row>
-    <row r="69" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H69" s="67">
         <v>9.1140638350711872E-2</v>
       </c>
@@ -8956,7 +8956,7 @@
       <c r="O69" s="51"/>
       <c r="P69" s="51"/>
     </row>
-    <row r="70" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H70" s="67">
         <v>0.1080445517892699</v>
       </c>
@@ -8972,7 +8972,7 @@
       <c r="O70" s="51"/>
       <c r="P70" s="51"/>
     </row>
-    <row r="71" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H71" s="67">
         <v>0.12497606826753388</v>
       </c>
@@ -8988,7 +8988,7 @@
       <c r="O71" s="51"/>
       <c r="P71" s="51"/>
     </row>
-    <row r="72" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H72" s="67">
         <v>0.14198052165390951</v>
       </c>
@@ -9004,7 +9004,7 @@
       <c r="O72" s="51"/>
       <c r="P72" s="51"/>
     </row>
-    <row r="73" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H73" s="67">
         <v>0.15874470475517963</v>
       </c>
@@ -9020,7 +9020,7 @@
       <c r="O73" s="51"/>
       <c r="P73" s="51"/>
     </row>
-    <row r="74" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H74" s="67">
         <v>0.17553747925232432</v>
       </c>
@@ -9036,7 +9036,7 @@
       <c r="O74" s="51"/>
       <c r="P74" s="51"/>
     </row>
-    <row r="75" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H75" s="67">
         <v>0.19240417629290971</v>
       </c>
@@ -9052,7 +9052,7 @@
       <c r="O75" s="51"/>
       <c r="P75" s="51"/>
     </row>
-    <row r="76" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H76" s="67">
         <v>0.20901220546271423</v>
       </c>
@@ -9068,7 +9068,7 @@
       <c r="O76" s="51"/>
       <c r="P76" s="51"/>
     </row>
-    <row r="77" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H77" s="67">
         <v>0.22582431925537669</v>
       </c>
@@ -9084,7 +9084,7 @@
       <c r="O77" s="51"/>
       <c r="P77" s="51"/>
     </row>
-    <row r="78" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H78" s="67">
         <v>0.24236713011424937</v>
       </c>
@@ -9100,7 +9100,7 @@
       <c r="O78" s="51"/>
       <c r="P78" s="51"/>
     </row>
-    <row r="79" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H79" s="67">
         <v>0.25891734586657894</v>
       </c>
@@ -9116,7 +9116,7 @@
       <c r="O79" s="51"/>
       <c r="P79" s="51"/>
     </row>
-    <row r="80" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H80" s="67">
         <v>0.27532743679881172</v>
       </c>
@@ -9132,7 +9132,7 @@
       <c r="O80" s="51"/>
       <c r="P80" s="51"/>
     </row>
-    <row r="81" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H81" s="67">
         <v>0.29164753874763422</v>
       </c>
@@ -9148,7 +9148,7 @@
       <c r="O81" s="51"/>
       <c r="P81" s="51"/>
     </row>
-    <row r="82" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H82" s="67">
         <v>0.30783618288424536</v>
       </c>
@@ -9164,7 +9164,7 @@
       <c r="O82" s="51"/>
       <c r="P82" s="51"/>
     </row>
-    <row r="83" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H83" s="67">
         <v>0.32384418347196781</v>
       </c>
@@ -9180,7 +9180,7 @@
       <c r="O83" s="51"/>
       <c r="P83" s="51"/>
     </row>
-    <row r="84" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H84" s="67">
         <v>0.33973325501759533</v>
       </c>
@@ -9196,7 +9196,7 @@
       <c r="O84" s="51"/>
       <c r="P84" s="51"/>
     </row>
-    <row r="85" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H85" s="67">
         <v>0.3553317399203158</v>
       </c>
@@ -9212,7 +9212,7 @@
       <c r="O85" s="51"/>
       <c r="P85" s="51"/>
     </row>
-    <row r="86" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H86" s="67">
         <v>0.37078429028268828</v>
       </c>
@@ -9228,7 +9228,7 @@
       <c r="O86" s="51"/>
       <c r="P86" s="51"/>
     </row>
-    <row r="87" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H87" s="67">
         <v>0.38613044476352726</v>
       </c>
@@ -9244,7 +9244,7 @@
       <c r="O87" s="51"/>
       <c r="P87" s="51"/>
     </row>
-    <row r="88" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H88" s="67">
         <v>0.4009921758963842</v>
       </c>
@@ -9260,7 +9260,7 @@
       <c r="O88" s="51"/>
       <c r="P88" s="51"/>
     </row>
-    <row r="89" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H89" s="67">
         <v>0.4156182923872962</v>
       </c>
@@ -9276,7 +9276,7 @@
       <c r="O89" s="51"/>
       <c r="P89" s="51"/>
     </row>
-    <row r="90" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H90" s="67">
         <v>0.42943502667027428</v>
       </c>
@@ -9292,7 +9292,7 @@
       <c r="O90" s="51"/>
       <c r="P90" s="51"/>
     </row>
-    <row r="91" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H91" s="67">
         <v>0.44289756776749095</v>
       </c>
@@ -9308,7 +9308,7 @@
       <c r="O91" s="51"/>
       <c r="P91" s="51"/>
     </row>
-    <row r="92" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H92" s="67">
         <v>0.45543894715911687</v>
       </c>
@@ -9324,7 +9324,7 @@
       <c r="O92" s="51"/>
       <c r="P92" s="51"/>
     </row>
-    <row r="93" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H93" s="67">
         <v>0.46783735943015631</v>
       </c>
@@ -9340,7 +9340,7 @@
       <c r="O93" s="51"/>
       <c r="P93" s="51"/>
     </row>
-    <row r="94" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H94" s="67">
         <v>0.47863400366300879</v>
       </c>
@@ -9356,7 +9356,7 @@
       <c r="O94" s="51"/>
       <c r="P94" s="51"/>
     </row>
-    <row r="95" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H95" s="67">
         <v>0.48872859410433517</v>
       </c>
@@ -9372,7 +9372,7 @@
       <c r="O95" s="51"/>
       <c r="P95" s="51"/>
     </row>
-    <row r="96" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H96" s="67">
         <v>0.49808648675762501</v>
       </c>
@@ -9388,7 +9388,7 @@
       <c r="O96" s="51"/>
       <c r="P96" s="51"/>
     </row>
-    <row r="97" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H97" s="67">
         <v>0.50622094031681064</v>
       </c>
@@ -9404,7 +9404,7 @@
       <c r="O97" s="51"/>
       <c r="P97" s="51"/>
     </row>
-    <row r="98" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H98" s="67">
         <v>0.51358901063162188</v>
       </c>
@@ -9420,7 +9420,7 @@
       <c r="O98" s="51"/>
       <c r="P98" s="51"/>
     </row>
-    <row r="99" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H99" s="67">
         <v>0.51988812196851808</v>
       </c>
@@ -9436,7 +9436,7 @@
       <c r="O99" s="51"/>
       <c r="P99" s="51"/>
     </row>
-    <row r="100" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H100" s="67">
         <v>0.52654380991188665</v>
       </c>
@@ -9452,7 +9452,7 @@
       <c r="O100" s="51"/>
       <c r="P100" s="51"/>
     </row>
-    <row r="101" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H101" s="67">
         <v>0.53210746291493216</v>
       </c>
@@ -9468,7 +9468,7 @@
       <c r="O101" s="51"/>
       <c r="P101" s="51"/>
     </row>
-    <row r="102" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H102" s="67">
         <v>0.53593356457098895</v>
       </c>
@@ -9484,7 +9484,7 @@
       <c r="O102" s="51"/>
       <c r="P102" s="51"/>
     </row>
-    <row r="103" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H103" s="67">
         <v>0.53837802652041589</v>
       </c>
@@ -9500,7 +9500,7 @@
       <c r="O103" s="51"/>
       <c r="P103" s="51"/>
     </row>
-    <row r="104" spans="8:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:16" x14ac:dyDescent="0.2">
       <c r="K104" s="51"/>
       <c r="L104" s="51"/>
       <c r="M104" s="51"/>

</xml_diff>

<commit_message>
Updated electricity price for 2024
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Jupyter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="867" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9447385-82B6-485D-A010-CC88D5C41EBC}"/>
+  <xr:revisionPtr revIDLastSave="869" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AEE3E2E-16B1-4D2E-B5F0-6B6EE1F3A37F}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -1039,9 +1039,6 @@
     <t>Gas constant</t>
   </si>
   <si>
-    <t>U.S. Energy Information Administration (Jan - Jun 2024) - industrial retail; GREET (2022)</t>
-  </si>
-  <si>
     <t>CEPCI 2021: 773.1
 CEPCI 2024: 800</t>
   </si>
@@ -1056,6 +1053,9 @@
   </si>
   <si>
     <t>Optimal j @ 8.2 c/kWh, Hawks model</t>
+  </si>
+  <si>
+    <t>U.S. Energy Information Administration (2024) - industrial retail; GREET (2022)</t>
   </si>
 </sst>
 </file>
@@ -5768,7 +5768,7 @@
         <v>152</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.5" x14ac:dyDescent="0.2">
@@ -6411,10 +6411,10 @@
         <v>78</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="P1" s="12" t="s">
         <v>24</v>
@@ -6513,7 +6513,7 @@
         <v>20</v>
       </c>
       <c r="Q3" s="42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="57" x14ac:dyDescent="0.2">
@@ -6567,7 +6567,7 @@
         <v>20</v>
       </c>
       <c r="Q4" s="24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="43" customFormat="1" ht="57" x14ac:dyDescent="0.2">
@@ -6637,8 +6637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6741,15 +6741,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="32">
-        <f>8.19/100</f>
-        <v>8.1900000000000001E-2</v>
+        <f>8.15/100</f>
+        <v>8.1500000000000003E-2</v>
       </c>
       <c r="C7" s="46" cm="1">
         <f t="array" ref="C7">[1]!Electricity_upstream_fuel_CO2/kWh_per_mmBtu</f>
         <v>414.10433834299573</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="71.25" x14ac:dyDescent="0.25">
@@ -6792,7 +6792,7 @@
       </c>
       <c r="B11" s="32">
         <f>B7</f>
-        <v>8.1900000000000001E-2</v>
+        <v>8.1500000000000003E-2</v>
       </c>
       <c r="C11" s="47">
         <f>C7</f>

</xml_diff>

<commit_message>
Updated details for the electricity cost update
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/shashwati_dacunha_austin_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="869" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AEE3E2E-16B1-4D2E-B5F0-6B6EE1F3A37F}"/>
+  <xr:revisionPtr revIDLastSave="876" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9735C05A-9411-4C73-B33C-760309F6EC63}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="16140" windowHeight="15585" activeTab="1" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -6345,8 +6345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCBDAF06-8365-4A5D-B76C-A5564B983B09}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -6504,7 +6504,7 @@
         <v>0.95</v>
       </c>
       <c r="N3" s="40">
-        <v>0.12379999999999999</v>
+        <v>0.1239</v>
       </c>
       <c r="O3" s="41">
         <v>472.1</v>
@@ -6558,7 +6558,7 @@
         <v>0.7</v>
       </c>
       <c r="N4" s="40">
-        <v>2.9170000000000001E-2</v>
+        <v>2.9219999999999999E-2</v>
       </c>
       <c r="O4" s="41">
         <v>435.9</v>
@@ -6637,8 +6637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BB50117-7FF7-46A9-9CB1-1D0EC2086168}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edited PSA capex default - not an acidic electrolyte
</commit_message>
<xml_diff>
--- a/Supplementary Workbook.xlsx
+++ b/Supplementary Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utexas-my.sharepoint.com/personal/scd2358_eid_utexas_edu/Documents/RCL Code/TEA/Streamlit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="879" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{774B3337-CF9C-4CCD-8B4F-2E4BFFAECAC2}"/>
+  <xr:revisionPtr revIDLastSave="880" documentId="8_{31750E0B-A732-4503-8EA8-2753BAB2D178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3683C90B-32F6-4F4F-BED8-7C1E345163B7}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="4200" windowWidth="21600" windowHeight="11235" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11235" xr2:uid="{A43CA30C-0C57-4CA9-B7DA-D833452F41BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants and assumptions" sheetId="2" r:id="rId1"/>
@@ -1622,6 +1622,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1633,9 +1636,6 @@
     </xf>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5699,7 +5699,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5814,8 +5814,8 @@
         <v>177</v>
       </c>
       <c r="C6" s="25">
-        <f>1.3*1989043*800/596.2</f>
-        <v>3469648.9768534047</v>
+        <f>1989043*800/596.2</f>
+        <v>2668960.7514256961</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>178</v>
@@ -5823,7 +5823,7 @@
       <c r="E6" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="73" t="s">
+      <c r="F6" s="69" t="s">
         <v>179</v>
       </c>
     </row>
@@ -6741,10 +6741,10 @@
       <c r="D3" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="69" t="s">
+      <c r="F3" s="70" t="s">
         <v>158</v>
       </c>
     </row>
@@ -6761,8 +6761,8 @@
       <c r="D4" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="70"/>
-      <c r="F4" s="69"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
@@ -7107,55 +7107,55 @@
       <c r="B14" s="52"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="72" t="s">
+      <c r="A17" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="H17" s="72" t="s">
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="H17" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="I17" s="72"/>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="72"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="73"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71" t="s">
+      <c r="B18" s="72"/>
+      <c r="C18" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71" t="s">
+      <c r="D18" s="72"/>
+      <c r="E18" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="F18" s="71"/>
+      <c r="F18" s="72"/>
       <c r="G18" s="58"/>
-      <c r="H18" s="71" t="s">
+      <c r="H18" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71" t="s">
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="L18" s="71"/>
-      <c r="M18" s="71"/>
-      <c r="N18" s="71" t="s">
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72"/>
     </row>
     <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="57" t="s">
@@ -8905,10 +8905,10 @@
       <c r="P62" s="51"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="H63" s="71" t="s">
+      <c r="H63" s="72" t="s">
         <v>130</v>
       </c>
-      <c r="I63" s="71"/>
+      <c r="I63" s="72"/>
       <c r="J63" s="65"/>
       <c r="K63" s="51"/>
       <c r="L63" s="51"/>

</xml_diff>